<commit_message>
Admin Interface for Transferred Samples WIP
</commit_message>
<xml_diff>
--- a/backend/fms_core/example_data/xlsx/Sample_transfer_v0.1.xlsx
+++ b/backend/fms_core/example_data/xlsx/Sample_transfer_v0.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jleblond/c3g/freezeman/backend/fms_core/example_data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30300353-CFD1-0E44-90BD-42F1BEBAF665}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BA4D8C-2FA8-8D48-881D-E95D90387CD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="1580" windowWidth="28800" windowHeight="16260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1580" windowWidth="28800" windowHeight="16260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleTransferTemplate" sheetId="1" r:id="rId1"/>
@@ -2196,8 +2196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD711"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2346,8 +2346,12 @@
       <c r="H10" s="29"/>
       <c r="I10" s="38"/>
       <c r="J10" s="22"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="10"/>
+      <c r="K10" s="23">
+        <v>20</v>
+      </c>
+      <c r="L10" s="10">
+        <v>9</v>
+      </c>
       <c r="M10" s="15"/>
       <c r="N10" s="11"/>
     </row>

</xml_diff>

<commit_message>
Add Sample Transfer action to interface
</commit_message>
<xml_diff>
--- a/backend/fms_core/example_data/xlsx/Sample_transfer_v0.1.xlsx
+++ b/backend/fms_core/example_data/xlsx/Sample_transfer_v0.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jleblond/c3g/freezeman/backend/fms_core/example_data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2D39FE-83B0-F943-89DE-76E1BECFA90F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F944AB0-6B60-2243-8029-49DDEC0263DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33900" yWindow="4060" windowWidth="28800" windowHeight="16260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37880" yWindow="1400" windowWidth="37060" windowHeight="20340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleTransferTemplate" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="411">
   <si>
     <t>#</t>
   </si>
@@ -1256,15 +1256,6 @@
   </si>
   <si>
     <t>Test J</t>
-  </si>
-  <si>
-    <t>EQ00421976</t>
-  </si>
-  <si>
-    <t>EQ00422030</t>
-  </si>
-  <si>
-    <t>Invalid Data</t>
   </si>
   <si>
     <t>EQ00432683</t>
@@ -2208,8 +2199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD711"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2344,7 +2335,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="32" t="s">
@@ -2375,29 +2366,19 @@
       <c r="A11" s="6">
         <v>3</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>411</v>
-      </c>
+      <c r="B11" s="10"/>
       <c r="C11" s="20"/>
-      <c r="D11" s="32" t="s">
-        <v>410</v>
-      </c>
+      <c r="D11" s="32"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="25"/>
       <c r="H11" s="29"/>
       <c r="I11" s="38"/>
       <c r="J11" s="22"/>
-      <c r="K11" s="23">
-        <v>7</v>
-      </c>
-      <c r="L11" s="10">
-        <v>6</v>
-      </c>
+      <c r="K11" s="23"/>
+      <c r="L11" s="10"/>
       <c r="M11" s="15"/>
-      <c r="N11" s="11" t="s">
-        <v>412</v>
-      </c>
+      <c r="N11" s="11"/>
     </row>
     <row r="12" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="6">

</xml_diff>

<commit_message>
Modify Sample Transfer to remove Volume column
</commit_message>
<xml_diff>
--- a/backend/fms_core/example_data/xlsx/Sample_transfer_v0.1.xlsx
+++ b/backend/fms_core/example_data/xlsx/Sample_transfer_v0.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jleblond/c3g/freezeman/backend/fms_core/example_data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F944AB0-6B60-2243-8029-49DDEC0263DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC96402-F321-7E4D-B9C5-6208AF68DB9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37880" yWindow="1400" windowWidth="37060" windowHeight="20340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,15 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="410">
   <si>
     <t>#</t>
   </si>
   <si>
     <t>Volume Used (uL)</t>
-  </si>
-  <si>
-    <t>Volume (uL)</t>
   </si>
   <si>
     <t>Comment</t>
@@ -2197,10 +2194,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD711"/>
+  <dimension ref="A1:AC711"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2215,104 +2212,100 @@
     <col min="8" max="9" width="33.5" customWidth="1"/>
     <col min="10" max="10" width="16.1640625" customWidth="1"/>
     <col min="11" max="11" width="16.5" customWidth="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="16.83203125" customWidth="1"/>
-    <col min="14" max="14" width="38.33203125" customWidth="1"/>
-    <col min="15" max="30" width="9.33203125" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" customWidth="1"/>
+    <col min="13" max="13" width="38.33203125" customWidth="1"/>
+    <col min="14" max="29" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="AD5" s="4"/>
-    </row>
-    <row r="6" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+      <c r="O5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="AC5" s="4"/>
+    </row>
+    <row r="6" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="AD6" s="4"/>
-    </row>
-    <row r="7" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+      <c r="O6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="AC6" s="4"/>
+    </row>
+    <row r="7" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>391</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="34" t="s">
         <v>392</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="E8" s="30" t="s">
         <v>393</v>
       </c>
-      <c r="E8" s="30" t="s">
-        <v>394</v>
-      </c>
       <c r="F8" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="G8" s="35" t="s">
         <v>398</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="H8" s="36" t="s">
+        <v>396</v>
+      </c>
+      <c r="I8" s="37" t="s">
+        <v>403</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>399</v>
-      </c>
-      <c r="H8" s="36" t="s">
-        <v>397</v>
-      </c>
-      <c r="I8" s="37" t="s">
-        <v>404</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>400</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L8" s="19" t="s">
+      <c r="L8" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="M8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="M8" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="N8" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>1</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="32" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G9" s="41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H9" s="28"/>
       <c r="I9" s="40"/>
@@ -2320,35 +2313,32 @@
       <c r="K9" s="23">
         <v>100</v>
       </c>
-      <c r="L9" s="10">
-        <v>95</v>
-      </c>
-      <c r="M9" s="15">
+      <c r="L9" s="15">
         <v>44197</v>
       </c>
-      <c r="N9" s="11" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+      <c r="M9" s="11" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>2</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="32" t="s">
+        <v>406</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>407</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>408</v>
-      </c>
       <c r="G10" s="41" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H10" s="29"/>
       <c r="I10" s="38"/>
@@ -2356,13 +2346,10 @@
       <c r="K10" s="23">
         <v>20</v>
       </c>
-      <c r="L10" s="10">
-        <v>9</v>
-      </c>
-      <c r="M10" s="15"/>
-      <c r="N10" s="11"/>
-    </row>
-    <row r="11" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+      <c r="L10" s="15"/>
+      <c r="M10" s="11"/>
+    </row>
+    <row r="11" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>3</v>
       </c>
@@ -2376,11 +2363,10 @@
       <c r="I11" s="38"/>
       <c r="J11" s="22"/>
       <c r="K11" s="23"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="11"/>
-    </row>
-    <row r="12" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+      <c r="L11" s="15"/>
+      <c r="M11" s="11"/>
+    </row>
+    <row r="12" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>4</v>
       </c>
@@ -2394,11 +2380,10 @@
       <c r="I12" s="38"/>
       <c r="J12" s="22"/>
       <c r="K12" s="23"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="11"/>
-    </row>
-    <row r="13" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+      <c r="L12" s="15"/>
+      <c r="M12" s="11"/>
+    </row>
+    <row r="13" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>5</v>
       </c>
@@ -2412,11 +2397,10 @@
       <c r="I13" s="38"/>
       <c r="J13" s="22"/>
       <c r="K13" s="23"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="11"/>
-    </row>
-    <row r="14" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+      <c r="L13" s="15"/>
+      <c r="M13" s="11"/>
+    </row>
+    <row r="14" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>6</v>
       </c>
@@ -2430,11 +2414,10 @@
       <c r="I14" s="38"/>
       <c r="J14" s="22"/>
       <c r="K14" s="23"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="11"/>
-    </row>
-    <row r="15" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+      <c r="L14" s="15"/>
+      <c r="M14" s="11"/>
+    </row>
+    <row r="15" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>7</v>
       </c>
@@ -2448,11 +2431,10 @@
       <c r="I15" s="38"/>
       <c r="J15" s="22"/>
       <c r="K15" s="23"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="11"/>
-    </row>
-    <row r="16" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+      <c r="L15" s="15"/>
+      <c r="M15" s="11"/>
+    </row>
+    <row r="16" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>8</v>
       </c>
@@ -2466,11 +2448,10 @@
       <c r="I16" s="38"/>
       <c r="J16" s="22"/>
       <c r="K16" s="23"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="11"/>
-    </row>
-    <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="L16" s="15"/>
+      <c r="M16" s="11"/>
+    </row>
+    <row r="17" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>9</v>
       </c>
@@ -2484,11 +2465,10 @@
       <c r="I17" s="38"/>
       <c r="J17" s="22"/>
       <c r="K17" s="23"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="11"/>
-    </row>
-    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="L17" s="15"/>
+      <c r="M17" s="11"/>
+    </row>
+    <row r="18" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>10</v>
       </c>
@@ -2502,11 +2482,10 @@
       <c r="I18" s="38"/>
       <c r="J18" s="22"/>
       <c r="K18" s="23"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="11"/>
-    </row>
-    <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="L18" s="15"/>
+      <c r="M18" s="11"/>
+    </row>
+    <row r="19" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>11</v>
       </c>
@@ -2520,11 +2499,10 @@
       <c r="I19" s="38"/>
       <c r="J19" s="22"/>
       <c r="K19" s="23"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="11"/>
-    </row>
-    <row r="20" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="L19" s="15"/>
+      <c r="M19" s="11"/>
+    </row>
+    <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>12</v>
       </c>
@@ -2538,11 +2516,10 @@
       <c r="I20" s="38"/>
       <c r="J20" s="22"/>
       <c r="K20" s="23"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="11"/>
-    </row>
-    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L20" s="15"/>
+      <c r="M20" s="11"/>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>13</v>
       </c>
@@ -2556,11 +2533,10 @@
       <c r="I21" s="38"/>
       <c r="J21" s="22"/>
       <c r="K21" s="23"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="11"/>
-    </row>
-    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L21" s="15"/>
+      <c r="M21" s="11"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>14</v>
       </c>
@@ -2574,11 +2550,10 @@
       <c r="I22" s="38"/>
       <c r="J22" s="22"/>
       <c r="K22" s="23"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="11"/>
-    </row>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L22" s="15"/>
+      <c r="M22" s="11"/>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>15</v>
       </c>
@@ -2592,11 +2567,10 @@
       <c r="I23" s="38"/>
       <c r="J23" s="22"/>
       <c r="K23" s="23"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="11"/>
-    </row>
-    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L23" s="15"/>
+      <c r="M23" s="11"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>16</v>
       </c>
@@ -2610,11 +2584,10 @@
       <c r="I24" s="38"/>
       <c r="J24" s="22"/>
       <c r="K24" s="23"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="11"/>
-    </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L24" s="15"/>
+      <c r="M24" s="11"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>17</v>
       </c>
@@ -2628,11 +2601,10 @@
       <c r="I25" s="38"/>
       <c r="J25" s="22"/>
       <c r="K25" s="23"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="11"/>
-    </row>
-    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L25" s="15"/>
+      <c r="M25" s="11"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>18</v>
       </c>
@@ -2646,11 +2618,10 @@
       <c r="I26" s="38"/>
       <c r="J26" s="22"/>
       <c r="K26" s="23"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="11"/>
-    </row>
-    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L26" s="15"/>
+      <c r="M26" s="11"/>
+    </row>
+    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>19</v>
       </c>
@@ -2664,11 +2635,10 @@
       <c r="I27" s="38"/>
       <c r="J27" s="22"/>
       <c r="K27" s="23"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="11"/>
-    </row>
-    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L27" s="15"/>
+      <c r="M27" s="11"/>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>20</v>
       </c>
@@ -2682,11 +2652,10 @@
       <c r="I28" s="38"/>
       <c r="J28" s="22"/>
       <c r="K28" s="23"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="11"/>
-    </row>
-    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L28" s="15"/>
+      <c r="M28" s="11"/>
+    </row>
+    <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>21</v>
       </c>
@@ -2700,11 +2669,10 @@
       <c r="I29" s="38"/>
       <c r="J29" s="22"/>
       <c r="K29" s="23"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="11"/>
-    </row>
-    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L29" s="15"/>
+      <c r="M29" s="11"/>
+    </row>
+    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>22</v>
       </c>
@@ -2718,11 +2686,10 @@
       <c r="I30" s="38"/>
       <c r="J30" s="22"/>
       <c r="K30" s="23"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="11"/>
-    </row>
-    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L30" s="15"/>
+      <c r="M30" s="11"/>
+    </row>
+    <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>23</v>
       </c>
@@ -2736,11 +2703,10 @@
       <c r="I31" s="38"/>
       <c r="J31" s="22"/>
       <c r="K31" s="23"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="11"/>
-    </row>
-    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L31" s="15"/>
+      <c r="M31" s="11"/>
+    </row>
+    <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>24</v>
       </c>
@@ -2754,11 +2720,10 @@
       <c r="I32" s="38"/>
       <c r="J32" s="22"/>
       <c r="K32" s="23"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="11"/>
-    </row>
-    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L32" s="15"/>
+      <c r="M32" s="11"/>
+    </row>
+    <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>25</v>
       </c>
@@ -2772,11 +2737,10 @@
       <c r="I33" s="38"/>
       <c r="J33" s="22"/>
       <c r="K33" s="23"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="11"/>
-    </row>
-    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L33" s="15"/>
+      <c r="M33" s="11"/>
+    </row>
+    <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>26</v>
       </c>
@@ -2790,11 +2754,10 @@
       <c r="I34" s="38"/>
       <c r="J34" s="22"/>
       <c r="K34" s="23"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="11"/>
-    </row>
-    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L34" s="15"/>
+      <c r="M34" s="11"/>
+    </row>
+    <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>27</v>
       </c>
@@ -2808,11 +2771,10 @@
       <c r="I35" s="38"/>
       <c r="J35" s="22"/>
       <c r="K35" s="23"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="11"/>
-    </row>
-    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L35" s="15"/>
+      <c r="M35" s="11"/>
+    </row>
+    <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>28</v>
       </c>
@@ -2826,11 +2788,10 @@
       <c r="I36" s="38"/>
       <c r="J36" s="22"/>
       <c r="K36" s="23"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="11"/>
-    </row>
-    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L36" s="15"/>
+      <c r="M36" s="11"/>
+    </row>
+    <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>29</v>
       </c>
@@ -2844,11 +2805,10 @@
       <c r="I37" s="38"/>
       <c r="J37" s="22"/>
       <c r="K37" s="23"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="11"/>
-    </row>
-    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L37" s="15"/>
+      <c r="M37" s="11"/>
+    </row>
+    <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>30</v>
       </c>
@@ -2862,11 +2822,10 @@
       <c r="I38" s="38"/>
       <c r="J38" s="22"/>
       <c r="K38" s="23"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="11"/>
-    </row>
-    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L38" s="15"/>
+      <c r="M38" s="11"/>
+    </row>
+    <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>31</v>
       </c>
@@ -2880,11 +2839,10 @@
       <c r="I39" s="38"/>
       <c r="J39" s="22"/>
       <c r="K39" s="23"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="11"/>
-    </row>
-    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L39" s="15"/>
+      <c r="M39" s="11"/>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>32</v>
       </c>
@@ -2898,11 +2856,10 @@
       <c r="I40" s="38"/>
       <c r="J40" s="22"/>
       <c r="K40" s="23"/>
-      <c r="L40" s="10"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="11"/>
-    </row>
-    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L40" s="15"/>
+      <c r="M40" s="11"/>
+    </row>
+    <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>33</v>
       </c>
@@ -2916,11 +2873,10 @@
       <c r="I41" s="38"/>
       <c r="J41" s="22"/>
       <c r="K41" s="23"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="11"/>
-    </row>
-    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L41" s="15"/>
+      <c r="M41" s="11"/>
+    </row>
+    <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>34</v>
       </c>
@@ -2934,11 +2890,10 @@
       <c r="I42" s="38"/>
       <c r="J42" s="22"/>
       <c r="K42" s="23"/>
-      <c r="L42" s="10"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="11"/>
-    </row>
-    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L42" s="15"/>
+      <c r="M42" s="11"/>
+    </row>
+    <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>35</v>
       </c>
@@ -2952,11 +2907,10 @@
       <c r="I43" s="38"/>
       <c r="J43" s="22"/>
       <c r="K43" s="23"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="11"/>
-    </row>
-    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L43" s="15"/>
+      <c r="M43" s="11"/>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>36</v>
       </c>
@@ -2970,11 +2924,10 @@
       <c r="I44" s="38"/>
       <c r="J44" s="22"/>
       <c r="K44" s="23"/>
-      <c r="L44" s="10"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="11"/>
-    </row>
-    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L44" s="15"/>
+      <c r="M44" s="11"/>
+    </row>
+    <row r="45" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>37</v>
       </c>
@@ -2988,11 +2941,10 @@
       <c r="I45" s="38"/>
       <c r="J45" s="22"/>
       <c r="K45" s="23"/>
-      <c r="L45" s="10"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="11"/>
-    </row>
-    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L45" s="15"/>
+      <c r="M45" s="11"/>
+    </row>
+    <row r="46" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>38</v>
       </c>
@@ -3006,11 +2958,10 @@
       <c r="I46" s="38"/>
       <c r="J46" s="22"/>
       <c r="K46" s="23"/>
-      <c r="L46" s="10"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="11"/>
-    </row>
-    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L46" s="15"/>
+      <c r="M46" s="11"/>
+    </row>
+    <row r="47" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>39</v>
       </c>
@@ -3024,11 +2975,10 @@
       <c r="I47" s="38"/>
       <c r="J47" s="22"/>
       <c r="K47" s="23"/>
-      <c r="L47" s="10"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="11"/>
-    </row>
-    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L47" s="15"/>
+      <c r="M47" s="11"/>
+    </row>
+    <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>40</v>
       </c>
@@ -3042,11 +2992,10 @@
       <c r="I48" s="38"/>
       <c r="J48" s="22"/>
       <c r="K48" s="23"/>
-      <c r="L48" s="10"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="11"/>
-    </row>
-    <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L48" s="15"/>
+      <c r="M48" s="11"/>
+    </row>
+    <row r="49" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>41</v>
       </c>
@@ -3060,11 +3009,10 @@
       <c r="I49" s="38"/>
       <c r="J49" s="22"/>
       <c r="K49" s="23"/>
-      <c r="L49" s="10"/>
-      <c r="M49" s="15"/>
-      <c r="N49" s="11"/>
-    </row>
-    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L49" s="15"/>
+      <c r="M49" s="11"/>
+    </row>
+    <row r="50" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>42</v>
       </c>
@@ -3078,11 +3026,10 @@
       <c r="I50" s="38"/>
       <c r="J50" s="22"/>
       <c r="K50" s="23"/>
-      <c r="L50" s="10"/>
-      <c r="M50" s="15"/>
-      <c r="N50" s="11"/>
-    </row>
-    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L50" s="15"/>
+      <c r="M50" s="11"/>
+    </row>
+    <row r="51" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>43</v>
       </c>
@@ -3096,11 +3043,10 @@
       <c r="I51" s="38"/>
       <c r="J51" s="22"/>
       <c r="K51" s="23"/>
-      <c r="L51" s="10"/>
-      <c r="M51" s="15"/>
-      <c r="N51" s="11"/>
-    </row>
-    <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L51" s="15"/>
+      <c r="M51" s="11"/>
+    </row>
+    <row r="52" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>44</v>
       </c>
@@ -3114,11 +3060,10 @@
       <c r="I52" s="38"/>
       <c r="J52" s="22"/>
       <c r="K52" s="23"/>
-      <c r="L52" s="10"/>
-      <c r="M52" s="15"/>
-      <c r="N52" s="11"/>
-    </row>
-    <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L52" s="15"/>
+      <c r="M52" s="11"/>
+    </row>
+    <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>45</v>
       </c>
@@ -3132,11 +3077,10 @@
       <c r="I53" s="38"/>
       <c r="J53" s="22"/>
       <c r="K53" s="23"/>
-      <c r="L53" s="10"/>
-      <c r="M53" s="15"/>
-      <c r="N53" s="11"/>
-    </row>
-    <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L53" s="15"/>
+      <c r="M53" s="11"/>
+    </row>
+    <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>46</v>
       </c>
@@ -3150,11 +3094,10 @@
       <c r="I54" s="38"/>
       <c r="J54" s="22"/>
       <c r="K54" s="23"/>
-      <c r="L54" s="10"/>
-      <c r="M54" s="15"/>
-      <c r="N54" s="11"/>
-    </row>
-    <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L54" s="15"/>
+      <c r="M54" s="11"/>
+    </row>
+    <row r="55" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="6">
         <v>47</v>
       </c>
@@ -3168,11 +3111,10 @@
       <c r="I55" s="38"/>
       <c r="J55" s="22"/>
       <c r="K55" s="23"/>
-      <c r="L55" s="10"/>
-      <c r="M55" s="15"/>
-      <c r="N55" s="11"/>
-    </row>
-    <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L55" s="15"/>
+      <c r="M55" s="11"/>
+    </row>
+    <row r="56" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
         <v>48</v>
       </c>
@@ -3186,11 +3128,10 @@
       <c r="I56" s="38"/>
       <c r="J56" s="22"/>
       <c r="K56" s="23"/>
-      <c r="L56" s="10"/>
-      <c r="M56" s="15"/>
-      <c r="N56" s="11"/>
-    </row>
-    <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L56" s="15"/>
+      <c r="M56" s="11"/>
+    </row>
+    <row r="57" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="6">
         <v>49</v>
       </c>
@@ -3204,11 +3145,10 @@
       <c r="I57" s="38"/>
       <c r="J57" s="22"/>
       <c r="K57" s="23"/>
-      <c r="L57" s="10"/>
-      <c r="M57" s="15"/>
-      <c r="N57" s="11"/>
-    </row>
-    <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L57" s="15"/>
+      <c r="M57" s="11"/>
+    </row>
+    <row r="58" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="6">
         <v>50</v>
       </c>
@@ -3222,11 +3162,10 @@
       <c r="I58" s="38"/>
       <c r="J58" s="22"/>
       <c r="K58" s="23"/>
-      <c r="L58" s="10"/>
-      <c r="M58" s="15"/>
-      <c r="N58" s="11"/>
-    </row>
-    <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L58" s="15"/>
+      <c r="M58" s="11"/>
+    </row>
+    <row r="59" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
         <v>51</v>
       </c>
@@ -3240,11 +3179,10 @@
       <c r="I59" s="38"/>
       <c r="J59" s="22"/>
       <c r="K59" s="23"/>
-      <c r="L59" s="10"/>
-      <c r="M59" s="15"/>
-      <c r="N59" s="11"/>
-    </row>
-    <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L59" s="15"/>
+      <c r="M59" s="11"/>
+    </row>
+    <row r="60" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
         <v>52</v>
       </c>
@@ -3258,11 +3196,10 @@
       <c r="I60" s="38"/>
       <c r="J60" s="22"/>
       <c r="K60" s="23"/>
-      <c r="L60" s="10"/>
-      <c r="M60" s="15"/>
-      <c r="N60" s="11"/>
-    </row>
-    <row r="61" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L60" s="15"/>
+      <c r="M60" s="11"/>
+    </row>
+    <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
         <v>53</v>
       </c>
@@ -3276,11 +3213,10 @@
       <c r="I61" s="38"/>
       <c r="J61" s="22"/>
       <c r="K61" s="23"/>
-      <c r="L61" s="10"/>
-      <c r="M61" s="15"/>
-      <c r="N61" s="11"/>
-    </row>
-    <row r="62" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L61" s="15"/>
+      <c r="M61" s="11"/>
+    </row>
+    <row r="62" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
         <v>54</v>
       </c>
@@ -3294,11 +3230,10 @@
       <c r="I62" s="38"/>
       <c r="J62" s="22"/>
       <c r="K62" s="23"/>
-      <c r="L62" s="10"/>
-      <c r="M62" s="15"/>
-      <c r="N62" s="11"/>
-    </row>
-    <row r="63" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L62" s="15"/>
+      <c r="M62" s="11"/>
+    </row>
+    <row r="63" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>55</v>
       </c>
@@ -3312,11 +3247,10 @@
       <c r="I63" s="38"/>
       <c r="J63" s="22"/>
       <c r="K63" s="23"/>
-      <c r="L63" s="10"/>
-      <c r="M63" s="15"/>
-      <c r="N63" s="11"/>
-    </row>
-    <row r="64" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L63" s="15"/>
+      <c r="M63" s="11"/>
+    </row>
+    <row r="64" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
         <v>56</v>
       </c>
@@ -3330,11 +3264,10 @@
       <c r="I64" s="38"/>
       <c r="J64" s="22"/>
       <c r="K64" s="23"/>
-      <c r="L64" s="10"/>
-      <c r="M64" s="15"/>
-      <c r="N64" s="11"/>
-    </row>
-    <row r="65" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L64" s="15"/>
+      <c r="M64" s="11"/>
+    </row>
+    <row r="65" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
         <v>57</v>
       </c>
@@ -3348,11 +3281,10 @@
       <c r="I65" s="38"/>
       <c r="J65" s="22"/>
       <c r="K65" s="23"/>
-      <c r="L65" s="10"/>
-      <c r="M65" s="15"/>
-      <c r="N65" s="11"/>
-    </row>
-    <row r="66" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L65" s="15"/>
+      <c r="M65" s="11"/>
+    </row>
+    <row r="66" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="6">
         <v>58</v>
       </c>
@@ -3366,11 +3298,10 @@
       <c r="I66" s="38"/>
       <c r="J66" s="22"/>
       <c r="K66" s="23"/>
-      <c r="L66" s="10"/>
-      <c r="M66" s="15"/>
-      <c r="N66" s="11"/>
-    </row>
-    <row r="67" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L66" s="15"/>
+      <c r="M66" s="11"/>
+    </row>
+    <row r="67" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="6">
         <v>59</v>
       </c>
@@ -3384,11 +3315,10 @@
       <c r="I67" s="38"/>
       <c r="J67" s="22"/>
       <c r="K67" s="23"/>
-      <c r="L67" s="10"/>
-      <c r="M67" s="15"/>
-      <c r="N67" s="11"/>
-    </row>
-    <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L67" s="15"/>
+      <c r="M67" s="11"/>
+    </row>
+    <row r="68" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="6">
         <v>60</v>
       </c>
@@ -3402,11 +3332,10 @@
       <c r="I68" s="38"/>
       <c r="J68" s="22"/>
       <c r="K68" s="23"/>
-      <c r="L68" s="10"/>
-      <c r="M68" s="15"/>
-      <c r="N68" s="11"/>
-    </row>
-    <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L68" s="15"/>
+      <c r="M68" s="11"/>
+    </row>
+    <row r="69" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="6">
         <v>61</v>
       </c>
@@ -3420,11 +3349,10 @@
       <c r="I69" s="38"/>
       <c r="J69" s="22"/>
       <c r="K69" s="23"/>
-      <c r="L69" s="10"/>
-      <c r="M69" s="15"/>
-      <c r="N69" s="11"/>
-    </row>
-    <row r="70" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L69" s="15"/>
+      <c r="M69" s="11"/>
+    </row>
+    <row r="70" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
         <v>62</v>
       </c>
@@ -3438,11 +3366,10 @@
       <c r="I70" s="38"/>
       <c r="J70" s="22"/>
       <c r="K70" s="23"/>
-      <c r="L70" s="10"/>
-      <c r="M70" s="15"/>
-      <c r="N70" s="11"/>
-    </row>
-    <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L70" s="15"/>
+      <c r="M70" s="11"/>
+    </row>
+    <row r="71" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="6">
         <v>63</v>
       </c>
@@ -3456,11 +3383,10 @@
       <c r="I71" s="38"/>
       <c r="J71" s="22"/>
       <c r="K71" s="23"/>
-      <c r="L71" s="10"/>
-      <c r="M71" s="15"/>
-      <c r="N71" s="11"/>
-    </row>
-    <row r="72" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L71" s="15"/>
+      <c r="M71" s="11"/>
+    </row>
+    <row r="72" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
         <v>64</v>
       </c>
@@ -3474,11 +3400,10 @@
       <c r="I72" s="38"/>
       <c r="J72" s="22"/>
       <c r="K72" s="23"/>
-      <c r="L72" s="10"/>
-      <c r="M72" s="15"/>
-      <c r="N72" s="11"/>
-    </row>
-    <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L72" s="15"/>
+      <c r="M72" s="11"/>
+    </row>
+    <row r="73" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="6">
         <v>65</v>
       </c>
@@ -3492,11 +3417,10 @@
       <c r="I73" s="38"/>
       <c r="J73" s="22"/>
       <c r="K73" s="23"/>
-      <c r="L73" s="10"/>
-      <c r="M73" s="15"/>
-      <c r="N73" s="11"/>
-    </row>
-    <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L73" s="15"/>
+      <c r="M73" s="11"/>
+    </row>
+    <row r="74" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="6">
         <v>66</v>
       </c>
@@ -3510,11 +3434,10 @@
       <c r="I74" s="38"/>
       <c r="J74" s="22"/>
       <c r="K74" s="23"/>
-      <c r="L74" s="10"/>
-      <c r="M74" s="15"/>
-      <c r="N74" s="11"/>
-    </row>
-    <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L74" s="15"/>
+      <c r="M74" s="11"/>
+    </row>
+    <row r="75" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="6">
         <v>67</v>
       </c>
@@ -3528,11 +3451,10 @@
       <c r="I75" s="38"/>
       <c r="J75" s="22"/>
       <c r="K75" s="23"/>
-      <c r="L75" s="10"/>
-      <c r="M75" s="15"/>
-      <c r="N75" s="11"/>
-    </row>
-    <row r="76" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L75" s="15"/>
+      <c r="M75" s="11"/>
+    </row>
+    <row r="76" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="6">
         <v>68</v>
       </c>
@@ -3546,11 +3468,10 @@
       <c r="I76" s="38"/>
       <c r="J76" s="22"/>
       <c r="K76" s="23"/>
-      <c r="L76" s="10"/>
-      <c r="M76" s="15"/>
-      <c r="N76" s="11"/>
-    </row>
-    <row r="77" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L76" s="15"/>
+      <c r="M76" s="11"/>
+    </row>
+    <row r="77" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="6">
         <v>69</v>
       </c>
@@ -3564,11 +3485,10 @@
       <c r="I77" s="38"/>
       <c r="J77" s="22"/>
       <c r="K77" s="23"/>
-      <c r="L77" s="10"/>
-      <c r="M77" s="15"/>
-      <c r="N77" s="11"/>
-    </row>
-    <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L77" s="15"/>
+      <c r="M77" s="11"/>
+    </row>
+    <row r="78" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="6">
         <v>70</v>
       </c>
@@ -3582,11 +3502,10 @@
       <c r="I78" s="38"/>
       <c r="J78" s="22"/>
       <c r="K78" s="23"/>
-      <c r="L78" s="10"/>
-      <c r="M78" s="15"/>
-      <c r="N78" s="11"/>
-    </row>
-    <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L78" s="15"/>
+      <c r="M78" s="11"/>
+    </row>
+    <row r="79" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="6">
         <v>71</v>
       </c>
@@ -3600,11 +3519,10 @@
       <c r="I79" s="38"/>
       <c r="J79" s="22"/>
       <c r="K79" s="23"/>
-      <c r="L79" s="10"/>
-      <c r="M79" s="15"/>
-      <c r="N79" s="11"/>
-    </row>
-    <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L79" s="15"/>
+      <c r="M79" s="11"/>
+    </row>
+    <row r="80" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="6">
         <v>72</v>
       </c>
@@ -3618,11 +3536,10 @@
       <c r="I80" s="38"/>
       <c r="J80" s="22"/>
       <c r="K80" s="23"/>
-      <c r="L80" s="10"/>
-      <c r="M80" s="15"/>
-      <c r="N80" s="11"/>
-    </row>
-    <row r="81" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L80" s="15"/>
+      <c r="M80" s="11"/>
+    </row>
+    <row r="81" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="6">
         <v>73</v>
       </c>
@@ -3636,11 +3553,10 @@
       <c r="I81" s="38"/>
       <c r="J81" s="22"/>
       <c r="K81" s="23"/>
-      <c r="L81" s="10"/>
-      <c r="M81" s="15"/>
-      <c r="N81" s="11"/>
-    </row>
-    <row r="82" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L81" s="15"/>
+      <c r="M81" s="11"/>
+    </row>
+    <row r="82" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="6">
         <v>74</v>
       </c>
@@ -3654,11 +3570,10 @@
       <c r="I82" s="38"/>
       <c r="J82" s="22"/>
       <c r="K82" s="23"/>
-      <c r="L82" s="10"/>
-      <c r="M82" s="15"/>
-      <c r="N82" s="11"/>
-    </row>
-    <row r="83" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L82" s="15"/>
+      <c r="M82" s="11"/>
+    </row>
+    <row r="83" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="6">
         <v>75</v>
       </c>
@@ -3672,11 +3587,10 @@
       <c r="I83" s="38"/>
       <c r="J83" s="22"/>
       <c r="K83" s="23"/>
-      <c r="L83" s="10"/>
-      <c r="M83" s="15"/>
-      <c r="N83" s="11"/>
-    </row>
-    <row r="84" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L83" s="15"/>
+      <c r="M83" s="11"/>
+    </row>
+    <row r="84" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="6">
         <v>76</v>
       </c>
@@ -3690,11 +3604,10 @@
       <c r="I84" s="38"/>
       <c r="J84" s="22"/>
       <c r="K84" s="23"/>
-      <c r="L84" s="10"/>
-      <c r="M84" s="15"/>
-      <c r="N84" s="11"/>
-    </row>
-    <row r="85" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L84" s="15"/>
+      <c r="M84" s="11"/>
+    </row>
+    <row r="85" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="6">
         <v>77</v>
       </c>
@@ -3708,11 +3621,10 @@
       <c r="I85" s="38"/>
       <c r="J85" s="22"/>
       <c r="K85" s="23"/>
-      <c r="L85" s="10"/>
-      <c r="M85" s="15"/>
-      <c r="N85" s="11"/>
-    </row>
-    <row r="86" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L85" s="15"/>
+      <c r="M85" s="11"/>
+    </row>
+    <row r="86" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="6">
         <v>78</v>
       </c>
@@ -3726,11 +3638,10 @@
       <c r="I86" s="38"/>
       <c r="J86" s="22"/>
       <c r="K86" s="23"/>
-      <c r="L86" s="10"/>
-      <c r="M86" s="15"/>
-      <c r="N86" s="11"/>
-    </row>
-    <row r="87" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L86" s="15"/>
+      <c r="M86" s="11"/>
+    </row>
+    <row r="87" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="6">
         <v>79</v>
       </c>
@@ -3744,11 +3655,10 @@
       <c r="I87" s="38"/>
       <c r="J87" s="22"/>
       <c r="K87" s="23"/>
-      <c r="L87" s="10"/>
-      <c r="M87" s="15"/>
-      <c r="N87" s="11"/>
-    </row>
-    <row r="88" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L87" s="15"/>
+      <c r="M87" s="11"/>
+    </row>
+    <row r="88" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="6">
         <v>80</v>
       </c>
@@ -3762,11 +3672,10 @@
       <c r="I88" s="38"/>
       <c r="J88" s="22"/>
       <c r="K88" s="23"/>
-      <c r="L88" s="10"/>
-      <c r="M88" s="15"/>
-      <c r="N88" s="11"/>
-    </row>
-    <row r="89" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L88" s="15"/>
+      <c r="M88" s="11"/>
+    </row>
+    <row r="89" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="6">
         <v>81</v>
       </c>
@@ -3780,11 +3689,10 @@
       <c r="I89" s="38"/>
       <c r="J89" s="22"/>
       <c r="K89" s="23"/>
-      <c r="L89" s="10"/>
-      <c r="M89" s="15"/>
-      <c r="N89" s="11"/>
-    </row>
-    <row r="90" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L89" s="15"/>
+      <c r="M89" s="11"/>
+    </row>
+    <row r="90" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="6">
         <v>82</v>
       </c>
@@ -3798,11 +3706,10 @@
       <c r="I90" s="38"/>
       <c r="J90" s="22"/>
       <c r="K90" s="23"/>
-      <c r="L90" s="10"/>
-      <c r="M90" s="15"/>
-      <c r="N90" s="11"/>
-    </row>
-    <row r="91" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L90" s="15"/>
+      <c r="M90" s="11"/>
+    </row>
+    <row r="91" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="6">
         <v>83</v>
       </c>
@@ -3816,11 +3723,10 @@
       <c r="I91" s="38"/>
       <c r="J91" s="22"/>
       <c r="K91" s="23"/>
-      <c r="L91" s="10"/>
-      <c r="M91" s="15"/>
-      <c r="N91" s="11"/>
-    </row>
-    <row r="92" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L91" s="15"/>
+      <c r="M91" s="11"/>
+    </row>
+    <row r="92" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="6">
         <v>84</v>
       </c>
@@ -3834,11 +3740,10 @@
       <c r="I92" s="38"/>
       <c r="J92" s="22"/>
       <c r="K92" s="23"/>
-      <c r="L92" s="10"/>
-      <c r="M92" s="15"/>
-      <c r="N92" s="11"/>
-    </row>
-    <row r="93" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L92" s="15"/>
+      <c r="M92" s="11"/>
+    </row>
+    <row r="93" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="6">
         <v>85</v>
       </c>
@@ -3852,11 +3757,10 @@
       <c r="I93" s="38"/>
       <c r="J93" s="22"/>
       <c r="K93" s="23"/>
-      <c r="L93" s="10"/>
-      <c r="M93" s="15"/>
-      <c r="N93" s="11"/>
-    </row>
-    <row r="94" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L93" s="15"/>
+      <c r="M93" s="11"/>
+    </row>
+    <row r="94" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="6">
         <v>86</v>
       </c>
@@ -3870,11 +3774,10 @@
       <c r="I94" s="38"/>
       <c r="J94" s="22"/>
       <c r="K94" s="23"/>
-      <c r="L94" s="10"/>
-      <c r="M94" s="15"/>
-      <c r="N94" s="11"/>
-    </row>
-    <row r="95" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L94" s="15"/>
+      <c r="M94" s="11"/>
+    </row>
+    <row r="95" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="6">
         <v>87</v>
       </c>
@@ -3888,11 +3791,10 @@
       <c r="I95" s="38"/>
       <c r="J95" s="22"/>
       <c r="K95" s="23"/>
-      <c r="L95" s="10"/>
-      <c r="M95" s="15"/>
-      <c r="N95" s="11"/>
-    </row>
-    <row r="96" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L95" s="15"/>
+      <c r="M95" s="11"/>
+    </row>
+    <row r="96" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="6">
         <v>88</v>
       </c>
@@ -3906,11 +3808,10 @@
       <c r="I96" s="38"/>
       <c r="J96" s="22"/>
       <c r="K96" s="23"/>
-      <c r="L96" s="10"/>
-      <c r="M96" s="15"/>
-      <c r="N96" s="11"/>
-    </row>
-    <row r="97" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L96" s="15"/>
+      <c r="M96" s="11"/>
+    </row>
+    <row r="97" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="6">
         <v>89</v>
       </c>
@@ -3924,11 +3825,10 @@
       <c r="I97" s="38"/>
       <c r="J97" s="22"/>
       <c r="K97" s="23"/>
-      <c r="L97" s="10"/>
-      <c r="M97" s="15"/>
-      <c r="N97" s="11"/>
-    </row>
-    <row r="98" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L97" s="15"/>
+      <c r="M97" s="11"/>
+    </row>
+    <row r="98" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="6">
         <v>90</v>
       </c>
@@ -3942,11 +3842,10 @@
       <c r="I98" s="38"/>
       <c r="J98" s="22"/>
       <c r="K98" s="23"/>
-      <c r="L98" s="10"/>
-      <c r="M98" s="15"/>
-      <c r="N98" s="11"/>
-    </row>
-    <row r="99" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L98" s="15"/>
+      <c r="M98" s="11"/>
+    </row>
+    <row r="99" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="6">
         <v>91</v>
       </c>
@@ -3960,11 +3859,10 @@
       <c r="I99" s="38"/>
       <c r="J99" s="22"/>
       <c r="K99" s="23"/>
-      <c r="L99" s="10"/>
-      <c r="M99" s="15"/>
-      <c r="N99" s="11"/>
-    </row>
-    <row r="100" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L99" s="15"/>
+      <c r="M99" s="11"/>
+    </row>
+    <row r="100" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="6">
         <v>92</v>
       </c>
@@ -3978,11 +3876,10 @@
       <c r="I100" s="38"/>
       <c r="J100" s="22"/>
       <c r="K100" s="23"/>
-      <c r="L100" s="10"/>
-      <c r="M100" s="15"/>
-      <c r="N100" s="11"/>
-    </row>
-    <row r="101" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L100" s="15"/>
+      <c r="M100" s="11"/>
+    </row>
+    <row r="101" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="6">
         <v>93</v>
       </c>
@@ -3996,11 +3893,10 @@
       <c r="I101" s="38"/>
       <c r="J101" s="22"/>
       <c r="K101" s="23"/>
-      <c r="L101" s="10"/>
-      <c r="M101" s="15"/>
-      <c r="N101" s="11"/>
-    </row>
-    <row r="102" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L101" s="15"/>
+      <c r="M101" s="11"/>
+    </row>
+    <row r="102" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="6">
         <v>94</v>
       </c>
@@ -4014,11 +3910,10 @@
       <c r="I102" s="38"/>
       <c r="J102" s="22"/>
       <c r="K102" s="23"/>
-      <c r="L102" s="10"/>
-      <c r="M102" s="15"/>
-      <c r="N102" s="11"/>
-    </row>
-    <row r="103" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L102" s="15"/>
+      <c r="M102" s="11"/>
+    </row>
+    <row r="103" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="6">
         <v>95</v>
       </c>
@@ -4032,11 +3927,10 @@
       <c r="I103" s="38"/>
       <c r="J103" s="22"/>
       <c r="K103" s="23"/>
-      <c r="L103" s="10"/>
-      <c r="M103" s="15"/>
-      <c r="N103" s="11"/>
-    </row>
-    <row r="104" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L103" s="15"/>
+      <c r="M103" s="11"/>
+    </row>
+    <row r="104" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6">
         <v>96</v>
       </c>
@@ -4050,18 +3944,17 @@
       <c r="I104" s="39"/>
       <c r="J104" s="24"/>
       <c r="K104" s="24"/>
-      <c r="L104" s="12"/>
-      <c r="M104" s="16"/>
-      <c r="N104" s="13"/>
-    </row>
-    <row r="105" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="106" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="107" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="108" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="109" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="110" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="111" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="112" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="L104" s="16"/>
+      <c r="M104" s="13"/>
+    </row>
+    <row r="105" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="106" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="107" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="108" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="109" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="110" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="111" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="112" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4710,2240 +4603,2240 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="14" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="17"/>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="18"/>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="17"/>
     </row>
     <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="17"/>
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="17"/>
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="17"/>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="17"/>
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="17"/>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>19</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>20</v>
       </c>
       <c r="C14" s="18"/>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>21</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>23</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>27</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="14" t="s">
         <v>29</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>31</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>33</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="14" t="s">
         <v>55</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="14" t="s">
         <v>59</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="14" t="s">
         <v>63</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="14" t="s">
         <v>65</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="14" t="s">
         <v>67</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="14" t="s">
         <v>69</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="14" t="s">
         <v>71</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="14" t="s">
         <v>73</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="14" t="s">
         <v>77</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B62" s="14" t="s">
         <v>91</v>
-      </c>
-      <c r="B62" s="14" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B63" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="B63" s="14" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B64" s="14" t="s">
         <v>95</v>
-      </c>
-      <c r="B64" s="14" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B65" s="14" t="s">
         <v>97</v>
-      </c>
-      <c r="B65" s="14" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B66" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="B66" s="14" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B67" s="14" t="s">
         <v>101</v>
-      </c>
-      <c r="B67" s="14" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B68" s="14" t="s">
         <v>103</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B69" s="14" t="s">
         <v>105</v>
-      </c>
-      <c r="B69" s="14" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B70" s="14" t="s">
         <v>107</v>
-      </c>
-      <c r="B70" s="14" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B71" s="14" t="s">
         <v>109</v>
-      </c>
-      <c r="B71" s="14" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B72" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="B72" s="14" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B73" s="14" t="s">
         <v>113</v>
-      </c>
-      <c r="B73" s="14" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B86" s="14" t="s">
         <v>127</v>
-      </c>
-      <c r="B86" s="14" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B87" s="14" t="s">
         <v>129</v>
-      </c>
-      <c r="B87" s="14" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B88" s="14" t="s">
         <v>131</v>
-      </c>
-      <c r="B88" s="14" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B89" s="14" t="s">
         <v>133</v>
-      </c>
-      <c r="B89" s="14" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B90" s="14" t="s">
         <v>135</v>
-      </c>
-      <c r="B90" s="14" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B91" s="14" t="s">
         <v>137</v>
-      </c>
-      <c r="B91" s="14" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B92" s="14" t="s">
         <v>139</v>
-      </c>
-      <c r="B92" s="14" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B93" s="14" t="s">
         <v>141</v>
-      </c>
-      <c r="B93" s="14" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B94" s="14" t="s">
         <v>143</v>
-      </c>
-      <c r="B94" s="14" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B95" s="14" t="s">
         <v>145</v>
-      </c>
-      <c r="B95" s="14" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B96" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="B96" s="14" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B97" s="14" t="s">
         <v>149</v>
-      </c>
-      <c r="B97" s="14" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B98" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B99" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B100" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B102" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B103" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B104" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B105" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B106" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B107" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B108" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B109" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B111" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B112" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="113" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B113" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="114" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B114" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="115" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B115" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="116" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B116" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="117" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B117" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="118" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B118" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="119" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B119" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="120" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B120" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="121" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B121" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="122" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B122" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="123" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B123" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="124" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B124" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="125" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B125" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="126" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B126" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="127" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B127" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="128" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B128" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="129" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B129" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="130" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B130" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="131" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B131" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="132" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B132" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="133" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B133" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="134" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B134" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="135" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B135" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="136" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B136" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="137" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B137" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="138" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B138" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="139" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B139" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="140" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B140" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="141" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B141" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="142" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B142" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="143" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B143" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="144" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B144" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="145" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B145" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="146" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B146" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="147" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B147" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="148" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B148" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="149" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B149" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="150" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B150" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="151" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B151" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="152" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B152" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="153" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B153" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="154" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B154" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="155" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B155" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="156" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B156" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="157" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B157" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="158" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B158" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="159" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B159" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="160" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B160" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="161" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B161" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="162" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B162" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="163" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B163" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="164" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B164" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="165" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B165" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="166" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B166" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="167" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B167" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="168" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B168" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="169" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B169" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="170" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B170" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="171" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B171" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="172" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B172" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="173" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B173" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="174" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B174" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="175" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B175" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="176" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B176" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="177" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B177" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="178" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B178" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="179" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B179" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="180" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B180" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="181" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B181" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="182" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B182" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="183" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B183" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="184" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B184" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="185" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B185" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="186" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B186" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="187" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B187" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="188" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B188" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="189" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B189" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="190" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B190" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="191" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B191" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="192" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B192" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="193" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B193" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="194" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B194" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="195" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B195" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="196" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B196" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="197" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B197" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="198" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B198" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="199" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B199" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="200" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B200" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="201" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B201" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="202" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B202" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="203" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B203" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="204" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B204" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="205" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B205" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="206" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B206" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="207" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B207" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="208" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B208" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="209" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B209" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="210" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B210" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="211" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B211" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="212" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B212" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="213" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B213" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="214" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B214" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="215" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B215" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="216" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B216" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="217" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B217" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="218" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B218" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="219" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B219" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="220" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B220" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="221" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B221" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="222" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B222" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="223" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B223" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="224" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B224" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="225" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B225" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="226" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B226" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="227" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B227" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="228" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B228" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="229" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B229" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="230" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B230" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="231" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B231" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="232" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B232" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="233" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B233" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="234" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B234" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="235" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B235" s="14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="236" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B236" s="14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="237" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B237" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="238" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B238" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="239" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B239" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="240" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B240" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="241" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B241" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="242" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B242" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="243" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B243" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="244" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B244" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="245" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B245" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="246" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B246" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="247" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B247" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="248" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B248" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="249" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B249" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="250" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B250" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="251" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B251" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="252" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B252" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="253" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B253" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="254" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B254" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="255" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B255" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="256" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B256" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="257" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B257" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="258" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B258" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="259" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B259" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="260" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B260" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="261" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B261" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="262" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B262" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="263" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B263" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="264" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B264" s="14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="265" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B265" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="266" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B266" s="14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="267" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B267" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="268" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B268" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="269" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B269" s="14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="270" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B270" s="14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="271" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B271" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="272" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B272" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="273" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B273" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="274" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B274" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="275" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B275" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="276" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B276" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="277" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B277" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="278" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B278" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="279" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B279" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="280" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B280" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="281" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B281" s="14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="282" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B282" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="283" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B283" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="284" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B284" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="285" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B285" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="286" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B286" s="14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="287" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B287" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="288" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B288" s="14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="289" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B289" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="290" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B290" s="14" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="291" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B291" s="14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="292" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B292" s="14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="293" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B293" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="294" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B294" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="295" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B295" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="296" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B296" s="14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="297" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B297" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="298" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B298" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="299" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B299" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="300" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B300" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="301" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B301" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="302" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B302" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="303" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B303" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="304" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B304" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="305" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B305" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="306" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B306" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="307" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B307" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="308" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B308" s="14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="309" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B309" s="14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="310" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B310" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="311" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B311" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="312" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B312" s="14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="313" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B313" s="14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="314" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B314" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="315" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B315" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="316" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B316" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="317" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B317" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="318" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B318" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="319" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B319" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="320" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B320" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="321" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B321" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="322" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B322" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="323" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B323" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="324" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B324" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="325" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B325" s="14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="326" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B326" s="14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="327" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B327" s="14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="328" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B328" s="14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="329" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B329" s="14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="330" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B330" s="14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="331" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B331" s="14" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="332" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B332" s="14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="333" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B333" s="14" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="334" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B334" s="14" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="335" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B335" s="14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="336" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B336" s="14" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="337" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B337" s="14" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="338" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B338" s="14" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="339" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B339" s="14" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="340" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B340" s="14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="341" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B341" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="342" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B342" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="343" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B343" s="14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="344" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B344" s="14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="345" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B345" s="14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="346" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B346" s="14" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="347" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B347" s="14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="348" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B348" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="349" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B349" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="350" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B350" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="351" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B351" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="352" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B352" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="353" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B353" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="354" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B354" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="355" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B355" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="356" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B356" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="357" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B357" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="358" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B358" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="359" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B359" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="360" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B360" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="361" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B361" s="14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="362" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B362" s="14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="363" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B363" s="14" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="364" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B364" s="14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="365" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B365" s="14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="366" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B366" s="14" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="367" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B367" s="14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="368" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B368" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="369" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B369" s="14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="370" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B370" s="14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="371" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B371" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="372" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B372" s="14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="373" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B373" s="14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="374" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B374" s="14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="375" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B375" s="14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="376" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B376" s="14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="377" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B377" s="14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="378" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B378" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="379" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B379" s="14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="380" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B380" s="14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="381" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B381" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="382" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B382" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="383" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B383" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="384" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B384" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="385" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B385" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="386" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>